<commit_message>
Second commit with DummyTest For Testing Jenkin
</commit_message>
<xml_diff>
--- a/insta.test/src/test/resources/data/RegInfo.xlsx
+++ b/insta.test/src/test/resources/data/RegInfo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t xml:space="preserve">Mr. No</t>
   </si>
@@ -196,6 +196,21 @@
   </si>
   <si>
     <t>DEP0085</t>
+  </si>
+  <si>
+    <t>ciphggd Dep</t>
+  </si>
+  <si>
+    <t>lkdpjno Dep</t>
+  </si>
+  <si>
+    <t>DEP0073</t>
+  </si>
+  <si>
+    <t>fjbkfdg Dep</t>
+  </si>
+  <si>
+    <t>DEP0074</t>
   </si>
 </sst>
 </file>
@@ -500,7 +515,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -596,6 +611,30 @@
         <v>57</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>